<commit_message>
Inseri uma forma de polimorfismo e alguns métodos de evitar erros
</commit_message>
<xml_diff>
--- a/saida.xlsx
+++ b/saida.xlsx
@@ -68,7 +68,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="3">
@@ -78,17 +78,17 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5.8</v>
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>